<commit_message>
Úprava funkcionality pro API.
Oprava chyby ve skriptu register.php
</commit_message>
<xml_diff>
--- a/tests/testovaci_scenare/testovaci_scenare.xlsx
+++ b/tests/testovaci_scenare/testovaci_scenare.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>TS01</t>
   </si>
@@ -108,7 +108,25 @@
     <t>Test ověřuje, zda-li  se uživatel může úspěšně přihlásit do systému s platnými údaji.</t>
   </si>
   <si>
-    <t xml:space="preserve">Přihlaseni </t>
+    <t>TS13</t>
+  </si>
+  <si>
+    <t>TS14</t>
+  </si>
+  <si>
+    <t>TS15</t>
+  </si>
+  <si>
+    <t>TS16</t>
+  </si>
+  <si>
+    <t>TS17</t>
+  </si>
+  <si>
+    <t>TS18</t>
+  </si>
+  <si>
+    <t>TS19</t>
   </si>
 </sst>
 </file>
@@ -180,14 +198,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -483,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D2:G16"/>
+  <dimension ref="D2:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -500,164 +518,218 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:7">
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" spans="4:7">
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="5" spans="4:7">
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="4:7">
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="4:7">
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="4:7" ht="30">
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="4:7" ht="30">
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="4:7" ht="30">
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="4:7" ht="30">
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="4:7">
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="4:7">
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="4:7">
+      <c r="D14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="4:7">
+      <c r="D15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="4:7">
+      <c r="D16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="4:7">
+      <c r="D17" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="4:7">
-      <c r="D14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="4:7">
-      <c r="D15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="4:7">
-      <c r="D16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="4:7">
+      <c r="D18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="4:7">
+      <c r="D19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="4:7">
+      <c r="D20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="4:7">
+      <c r="D21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="4:7">
+      <c r="D22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="4:7">
+      <c r="D23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Uprava testovaci struktury. Doimplementovano logovani.
</commit_message>
<xml_diff>
--- a/tests/testovaci_scenare/testovaci_scenare.xlsx
+++ b/tests/testovaci_scenare/testovaci_scenare.xlsx
@@ -158,7 +158,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,6 +168,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -199,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -211,6 +217,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -510,7 +519,7 @@
   <dimension ref="D2:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -532,7 +541,7 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="4:5">
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -540,7 +549,7 @@
       </c>
     </row>
     <row r="5" spans="4:5">
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -548,7 +557,7 @@
       </c>
     </row>
     <row r="6" spans="4:5">
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="2" t="s">

</xml_diff>